<commit_message>
paar Änderungen an der CMakeLists.txt von gestern; Excel der Bestellung vom 01.Juni angepasst (alles angekommen :)))
</commit_message>
<xml_diff>
--- a/LCSC_Bestellung_01_Juni21.xlsx
+++ b/LCSC_Bestellung_01_Juni21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4551c9f81874734a/Documents/Projekte/Speed_sensor/speed_sensor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nils_\Documents\Projects\speed_sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="11_AD4DB114E441178AC67DF4151E15CED6683EDF1D" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B625633D-E269-47B8-93E8-B0B2EE47931D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDD8F9F-2E40-4201-ABCC-E53348E87496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="2664" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>LCSC part no.</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>C319196</t>
+  </si>
+  <si>
+    <t>angekommen</t>
   </si>
 </sst>
 </file>
@@ -154,12 +157,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -183,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -201,6 +210,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -481,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,9 +507,10 @@
     <col min="4" max="4" width="30.88671875" style="6" customWidth="1"/>
     <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -513,8 +526,11 @@
       <c r="F1" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -530,8 +546,11 @@
       <c r="F2" s="6">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -550,8 +569,11 @@
       <c r="F3" s="6">
         <v>1000</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -567,8 +589,11 @@
       <c r="F4" s="6">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -584,8 +609,11 @@
       <c r="F5" s="6">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -601,8 +629,11 @@
       <c r="F6" s="6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -618,8 +649,11 @@
       <c r="F7" s="6">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -635,8 +669,11 @@
       <c r="F9" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -652,8 +689,11 @@
       <c r="F11" s="6">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -669,8 +709,11 @@
       <c r="F12" s="6">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -686,8 +729,11 @@
       <c r="F13" s="6">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -703,8 +749,11 @@
       <c r="F15" s="6">
         <v>500</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -718,6 +767,9 @@
         <v>603</v>
       </c>
       <c r="F16" s="6">
+        <v>20</v>
+      </c>
+      <c r="G16" s="9">
         <v>20</v>
       </c>
     </row>

</xml_diff>